<commit_message>
test de création des colonnes supplémentaire pour la prépublication (données non chragée. Bug couleur sur colonne existante )
</commit_message>
<xml_diff>
--- a/src/main/resources/template-segur-requirement-export.xlsx
+++ b/src/main/resources/template-segur-requirement-export.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjuillard\Documents\Segur-Squash\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjuillard\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B9DABDD-D342-47B7-B53B-4CBB6EB0E047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3939867F-AF15-449E-9074-103E5EFFDB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{07F62732-3230-4871-935B-304D9A8AE51A}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Preuve</t>
   </si>
@@ -228,13 +228,7 @@
     <t>bon pour publication</t>
   </si>
   <si>
-    <t>référence exigence</t>
-  </si>
-  <si>
     <t>référence cas de test</t>
-  </si>
-  <si>
-    <t>référence exigence socle</t>
   </si>
   <si>
     <t>points de vérification</t>
@@ -804,11 +798,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A72A65-80DB-4F9C-B4D9-9208DB126119}">
   <sheetPr codeName="Feuil5"/>
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="60" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.25"/>
@@ -844,11 +838,10 @@
     <col min="29" max="29" width="40.6640625" style="21" customWidth="1"/>
     <col min="30" max="30" width="12.33203125" style="21" customWidth="1"/>
     <col min="31" max="31" width="20.6640625" style="21" customWidth="1"/>
-    <col min="32" max="36" width="28.1640625" style="15" customWidth="1"/>
-    <col min="37" max="16384" width="11.6640625" style="15"/>
+    <col min="32" max="16384" width="11.6640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="14" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" s="14" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>13</v>
       </c>
@@ -942,23 +935,8 @@
       <c r="AE1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="AF1" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG1" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH1" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI1" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="AJ1" s="23" t="s">
-        <v>48</v>
-      </c>
     </row>
-    <row r="2" spans="1:36" s="14" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" s="14" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1051,21 +1029,6 @@
       </c>
       <c r="AE2" s="9">
         <v>31</v>
-      </c>
-      <c r="AF2" s="9">
-        <v>32</v>
-      </c>
-      <c r="AG2" s="9">
-        <v>33</v>
-      </c>
-      <c r="AH2" s="9">
-        <v>34</v>
-      </c>
-      <c r="AI2" s="9">
-        <v>35</v>
-      </c>
-      <c r="AJ2" s="9">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1144,13 +1107,13 @@
         <v>44</v>
       </c>
       <c r="P1" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" s="23" t="s">
         <v>46</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="R1" s="23" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="7" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add hyperlink to requirement number
</commit_message>
<xml_diff>
--- a/src/main/resources/template-segur-requirement-export.xlsx
+++ b/src/main/resources/template-segur-requirement-export.xlsx
@@ -330,12 +330,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="37">
+  <fonts count="38">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -425,10 +425,76 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -440,23 +506,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -470,18 +530,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -493,41 +553,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -539,19 +569,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -560,25 +586,6 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
@@ -629,181 +636,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,17 +839,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -850,8 +853,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -871,13 +874,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -900,23 +907,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -925,47 +932,47 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -974,110 +981,110 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1175,6 +1182,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1532,7 +1543,7 @@
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.3" defaultRowHeight="15.75" outlineLevelRow="1"/>
@@ -1596,73 +1607,73 @@
       <c r="H1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="L1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="M1" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="O1" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="R1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="S1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="35" t="s">
+      <c r="T1" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="U1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="35" t="s">
+      <c r="V1" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="34" t="s">
+      <c r="W1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="35" t="s">
+      <c r="X1" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="34" t="s">
+      <c r="Y1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="35" t="s">
+      <c r="Z1" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="34" t="s">
+      <c r="AA1" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="35" t="s">
+      <c r="AB1" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="34" t="s">
+      <c r="AC1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="35" t="s">
+      <c r="AD1" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="34" t="s">
+      <c r="AE1" s="35" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1688,60 +1699,60 @@
       <c r="G2" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="M2" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="39" t="s">
+      <c r="N2" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="38" t="s">
+      <c r="O2" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="38" t="s">
+      <c r="P2" s="40"/>
+      <c r="Q2" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="R2" s="39"/>
-      <c r="S2" s="38" t="s">
+      <c r="R2" s="40"/>
+      <c r="S2" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="T2" s="39"/>
-      <c r="U2" s="38" t="s">
+      <c r="T2" s="40"/>
+      <c r="U2" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="39"/>
-      <c r="W2" s="38" t="s">
+      <c r="V2" s="40"/>
+      <c r="W2" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="39"/>
-      <c r="Y2" s="38" t="s">
+      <c r="X2" s="40"/>
+      <c r="Y2" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="Z2" s="39"/>
-      <c r="AA2" s="38" t="s">
+      <c r="Z2" s="40"/>
+      <c r="AA2" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="AB2" s="39"/>
-      <c r="AC2" s="38" t="s">
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="AD2" s="39"/>
-      <c r="AE2" s="38" t="s">
+      <c r="AD2" s="40"/>
+      <c r="AE2" s="39" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1749,6 +1760,9 @@
   <autoFilter ref="A1:AF2">
     <extLst/>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="INS.01"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>